<commit_message>
update excel update controller
</commit_message>
<xml_diff>
--- a/Web/wwwroot/Files/Template/EditPersonnel_Template.xlsx
+++ b/Web/wwwroot/Files/Template/EditPersonnel_Template.xlsx
@@ -1,48 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\Kosha\Doc\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Erfan Shayegh\source\repos\IEfiwm\SalaryManagment\Web\wwwroot\Files\Template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40550068-1093-4F7E-9175-FAA386C3809A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5FE26C0-C301-4DDC-8460-77D80A186ADB}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13464" windowHeight="5376"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>کدملی</t>
   </si>
   <si>
-    <t>پایه سنوات</t>
-  </si>
-  <si>
     <t>حقوق ماهانه</t>
   </si>
   <si>
@@ -59,16 +45,51 @@
   </si>
   <si>
     <t>حقوق روزانه</t>
+  </si>
+  <si>
+    <t xml:space="preserve">کد بیمه </t>
+  </si>
+  <si>
+    <t>موبایل</t>
+  </si>
+  <si>
+    <t>شماره حساب</t>
+  </si>
+  <si>
+    <t>شماره شبا</t>
+  </si>
+  <si>
+    <t>تعداد اولاد</t>
+  </si>
+  <si>
+    <t>تعداد اولاد مشمول</t>
+  </si>
+  <si>
+    <t>پایه سنوات ماهانه</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -83,8 +104,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39997558519241921"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -97,14 +117,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -416,52 +446,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8B7A546-E328-402C-879C-059842A6659F}">
-  <dimension ref="A1:H1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N1"/>
   <sheetViews>
-    <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD2"/>
+    <sheetView rightToLeft="1" tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.77734375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.44140625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" customWidth="1"/>
+    <col min="2" max="14" width="20.77734375" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:14" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>